<commit_message>
fix GD_KhachHang and GD_SanPham
</commit_message>
<xml_diff>
--- a/LuuFile_Excel/DanhSach.xlsx
+++ b/LuuFile_Excel/DanhSach.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="330" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="330" uniqueCount="108">
   <si>
     <t/>
   </si>
@@ -44,13 +44,13 @@
     <t>Hình ảnh</t>
   </si>
   <si>
-    <t>SP001</t>
-  </si>
-  <si>
-    <t>Bia Tiger nâu</t>
-  </si>
-  <si>
-    <t>20-09-2023</t>
+    <t>SP002</t>
+  </si>
+  <si>
+    <t>Bia Tiger bạc</t>
+  </si>
+  <si>
+    <t>02-10-2023</t>
   </si>
   <si>
     <t>Bia</t>
@@ -59,45 +59,21 @@
     <t>Lon</t>
   </si>
   <si>
-    <t>D:\BaiTapLonPTUD_NHOM4\image\BiaTigerNau001.jpg</t>
-  </si>
-  <si>
-    <t>SP002</t>
-  </si>
-  <si>
-    <t>Bia Tiger bạc</t>
-  </si>
-  <si>
-    <t>02-10-2023</t>
-  </si>
-  <si>
     <t>D:\BaiTapLonPTUD_NHOM4\image\BiaTigerBac002.jpg</t>
   </si>
   <si>
-    <t>SP003</t>
-  </si>
-  <si>
-    <t>Nước ngọt pepsi</t>
-  </si>
-  <si>
-    <t>22-09-2023</t>
+    <t>SP004</t>
+  </si>
+  <si>
+    <t>Nước ngọt Coca cola</t>
+  </si>
+  <si>
+    <t>17-08-2023</t>
   </si>
   <si>
     <t>Nước ngọt</t>
   </si>
   <si>
-    <t>D:\BaiTapLonPTUD_NHOM4\image\NuocNgotPepsi003.jpg</t>
-  </si>
-  <si>
-    <t>SP004</t>
-  </si>
-  <si>
-    <t>Nước ngọt Coca cola</t>
-  </si>
-  <si>
-    <t>17-08-2023</t>
-  </si>
-  <si>
     <t>D:\BaiTapLonPTUD_NHOM4\image\NuocNgotCoca004.jpg</t>
   </si>
   <si>
@@ -345,6 +321,21 @@
   </si>
   <si>
     <t>D:\BaiTapLonPTUD_NHOM4\image\TraGungDaNong026.jpg</t>
+  </si>
+  <si>
+    <t>SP027</t>
+  </si>
+  <si>
+    <t>Nô mai</t>
+  </si>
+  <si>
+    <t>22-04-2024</t>
+  </si>
+  <si>
+    <t>SP028</t>
+  </si>
+  <si>
+    <t>fff</t>
   </si>
 </sst>
 </file>
@@ -441,13 +432,13 @@
         <v>13</v>
       </c>
       <c r="F4" t="n">
-        <v>10000.0</v>
+        <v>17000.0</v>
       </c>
       <c r="G4" t="s">
         <v>14</v>
       </c>
       <c r="H4" t="n">
-        <v>18000.0</v>
+        <v>10000.0</v>
       </c>
       <c r="I4" t="s">
         <v>15</v>
@@ -467,19 +458,19 @@
         <v>18</v>
       </c>
       <c r="E5" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="F5" t="n">
-        <v>17000.0</v>
+        <v>11000.0</v>
       </c>
       <c r="G5" t="s">
         <v>14</v>
       </c>
       <c r="H5" t="n">
-        <v>10000.0</v>
+        <v>12000.0</v>
       </c>
       <c r="I5" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="6">
@@ -487,25 +478,25 @@
         <v>3.0</v>
       </c>
       <c r="B6" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C6" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D6" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E6" t="s">
-        <v>23</v>
+        <v>13</v>
       </c>
       <c r="F6" t="n">
-        <v>10500.0</v>
+        <v>12000.0</v>
       </c>
       <c r="G6" t="s">
         <v>14</v>
       </c>
       <c r="H6" t="n">
-        <v>23000.0</v>
+        <v>9000.0</v>
       </c>
       <c r="I6" t="s">
         <v>24</v>
@@ -525,16 +516,16 @@
         <v>27</v>
       </c>
       <c r="E7" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="F7" t="n">
-        <v>11000.0</v>
+        <v>10000.0</v>
       </c>
       <c r="G7" t="s">
         <v>14</v>
       </c>
       <c r="H7" t="n">
-        <v>12000.0</v>
+        <v>15000.0</v>
       </c>
       <c r="I7" t="s">
         <v>28</v>
@@ -554,19 +545,19 @@
         <v>31</v>
       </c>
       <c r="E8" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="F8" t="n">
         <v>12000.0</v>
       </c>
       <c r="G8" t="s">
-        <v>14</v>
+        <v>32</v>
       </c>
       <c r="H8" t="n">
-        <v>9000.0</v>
+        <v>6000.0</v>
       </c>
       <c r="I8" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="9">
@@ -574,28 +565,28 @@
         <v>6.0</v>
       </c>
       <c r="B9" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C9" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D9" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E9" t="s">
-        <v>23</v>
+        <v>37</v>
       </c>
       <c r="F9" t="n">
-        <v>10000.0</v>
+        <v>90000.0</v>
       </c>
       <c r="G9" t="s">
-        <v>14</v>
+        <v>38</v>
       </c>
       <c r="H9" t="n">
-        <v>15000.0</v>
+        <v>5000.0</v>
       </c>
       <c r="I9" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
     </row>
     <row r="10">
@@ -603,28 +594,28 @@
         <v>7.0</v>
       </c>
       <c r="B10" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="C10" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="D10" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="E10" t="s">
-        <v>23</v>
+        <v>37</v>
       </c>
       <c r="F10" t="n">
-        <v>12000.0</v>
+        <v>40000.0</v>
       </c>
       <c r="G10" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="H10" t="n">
-        <v>6000.0</v>
+        <v>2000.0</v>
       </c>
       <c r="I10" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
     </row>
     <row r="11">
@@ -632,25 +623,25 @@
         <v>8.0</v>
       </c>
       <c r="B11" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="C11" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="D11" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="E11" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="F11" t="n">
-        <v>90000.0</v>
+        <v>35000.0</v>
       </c>
       <c r="G11" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="H11" t="n">
-        <v>4960.0</v>
+        <v>600.0</v>
       </c>
       <c r="I11" t="s">
         <v>47</v>
@@ -667,19 +658,19 @@
         <v>49</v>
       </c>
       <c r="D12" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="E12" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="F12" t="n">
-        <v>40000.0</v>
+        <v>90000.0</v>
       </c>
       <c r="G12" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="H12" t="n">
-        <v>2000.0</v>
+        <v>700.0</v>
       </c>
       <c r="I12" t="s">
         <v>51</v>
@@ -696,22 +687,22 @@
         <v>53</v>
       </c>
       <c r="D13" t="s">
+        <v>46</v>
+      </c>
+      <c r="E13" t="s">
+        <v>37</v>
+      </c>
+      <c r="F13" t="n">
+        <v>170000.0</v>
+      </c>
+      <c r="G13" t="s">
+        <v>42</v>
+      </c>
+      <c r="H13" t="n">
+        <v>200.0</v>
+      </c>
+      <c r="I13" t="s">
         <v>54</v>
-      </c>
-      <c r="E13" t="s">
-        <v>45</v>
-      </c>
-      <c r="F13" t="n">
-        <v>35000.0</v>
-      </c>
-      <c r="G13" t="s">
-        <v>50</v>
-      </c>
-      <c r="H13" t="n">
-        <v>590.0</v>
-      </c>
-      <c r="I13" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="14">
@@ -719,28 +710,28 @@
         <v>11.0</v>
       </c>
       <c r="B14" t="s">
+        <v>55</v>
+      </c>
+      <c r="C14" t="s">
         <v>56</v>
       </c>
-      <c r="C14" t="s">
+      <c r="D14" t="s">
         <v>57</v>
       </c>
-      <c r="D14" t="s">
+      <c r="E14" t="s">
+        <v>37</v>
+      </c>
+      <c r="F14" t="n">
+        <v>210000.0</v>
+      </c>
+      <c r="G14" t="s">
+        <v>42</v>
+      </c>
+      <c r="H14" t="n">
+        <v>800.0</v>
+      </c>
+      <c r="I14" t="s">
         <v>58</v>
-      </c>
-      <c r="E14" t="s">
-        <v>45</v>
-      </c>
-      <c r="F14" t="n">
-        <v>90000.0</v>
-      </c>
-      <c r="G14" t="s">
-        <v>50</v>
-      </c>
-      <c r="H14" t="n">
-        <v>690.0</v>
-      </c>
-      <c r="I14" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="15">
@@ -748,25 +739,25 @@
         <v>12.0</v>
       </c>
       <c r="B15" t="s">
+        <v>59</v>
+      </c>
+      <c r="C15" t="s">
         <v>60</v>
       </c>
-      <c r="C15" t="s">
+      <c r="D15" t="s">
         <v>61</v>
       </c>
-      <c r="D15" t="s">
-        <v>54</v>
-      </c>
       <c r="E15" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="F15" t="n">
-        <v>170000.0</v>
+        <v>80000.0</v>
       </c>
       <c r="G15" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="H15" t="n">
-        <v>200.0</v>
+        <v>400.0</v>
       </c>
       <c r="I15" t="s">
         <v>62</v>
@@ -786,16 +777,16 @@
         <v>65</v>
       </c>
       <c r="E16" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="F16" t="n">
-        <v>210000.0</v>
+        <v>150000.0</v>
       </c>
       <c r="G16" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="H16" t="n">
-        <v>800.0</v>
+        <v>250.0</v>
       </c>
       <c r="I16" t="s">
         <v>66</v>
@@ -815,16 +806,16 @@
         <v>69</v>
       </c>
       <c r="E17" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="F17" t="n">
-        <v>80000.0</v>
+        <v>120000.0</v>
       </c>
       <c r="G17" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="H17" t="n">
-        <v>400.0</v>
+        <v>1000.0</v>
       </c>
       <c r="I17" t="s">
         <v>70</v>
@@ -841,22 +832,22 @@
         <v>72</v>
       </c>
       <c r="D18" t="s">
+        <v>61</v>
+      </c>
+      <c r="E18" t="s">
+        <v>37</v>
+      </c>
+      <c r="F18" t="n">
+        <v>200000.0</v>
+      </c>
+      <c r="G18" t="s">
+        <v>42</v>
+      </c>
+      <c r="H18" t="n">
+        <v>180.0</v>
+      </c>
+      <c r="I18" t="s">
         <v>73</v>
-      </c>
-      <c r="E18" t="s">
-        <v>45</v>
-      </c>
-      <c r="F18" t="n">
-        <v>150000.0</v>
-      </c>
-      <c r="G18" t="s">
-        <v>50</v>
-      </c>
-      <c r="H18" t="n">
-        <v>250.0</v>
-      </c>
-      <c r="I18" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="19">
@@ -864,28 +855,28 @@
         <v>16.0</v>
       </c>
       <c r="B19" t="s">
+        <v>74</v>
+      </c>
+      <c r="C19" t="s">
         <v>75</v>
       </c>
-      <c r="C19" t="s">
+      <c r="D19" t="s">
+        <v>65</v>
+      </c>
+      <c r="E19" t="s">
+        <v>37</v>
+      </c>
+      <c r="F19" t="n">
+        <v>190000.0</v>
+      </c>
+      <c r="G19" t="s">
+        <v>42</v>
+      </c>
+      <c r="H19" t="n">
+        <v>200.0</v>
+      </c>
+      <c r="I19" t="s">
         <v>76</v>
-      </c>
-      <c r="D19" t="s">
-        <v>77</v>
-      </c>
-      <c r="E19" t="s">
-        <v>45</v>
-      </c>
-      <c r="F19" t="n">
-        <v>120000.0</v>
-      </c>
-      <c r="G19" t="s">
-        <v>50</v>
-      </c>
-      <c r="H19" t="n">
-        <v>1000.0</v>
-      </c>
-      <c r="I19" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="20">
@@ -893,28 +884,28 @@
         <v>17.0</v>
       </c>
       <c r="B20" t="s">
+        <v>77</v>
+      </c>
+      <c r="C20" t="s">
+        <v>78</v>
+      </c>
+      <c r="D20" t="s">
+        <v>65</v>
+      </c>
+      <c r="E20" t="s">
+        <v>37</v>
+      </c>
+      <c r="F20" t="n">
+        <v>240000.0</v>
+      </c>
+      <c r="G20" t="s">
+        <v>42</v>
+      </c>
+      <c r="H20" t="n">
+        <v>100.0</v>
+      </c>
+      <c r="I20" t="s">
         <v>79</v>
-      </c>
-      <c r="C20" t="s">
-        <v>80</v>
-      </c>
-      <c r="D20" t="s">
-        <v>69</v>
-      </c>
-      <c r="E20" t="s">
-        <v>45</v>
-      </c>
-      <c r="F20" t="n">
-        <v>200000.0</v>
-      </c>
-      <c r="G20" t="s">
-        <v>50</v>
-      </c>
-      <c r="H20" t="n">
-        <v>180.0</v>
-      </c>
-      <c r="I20" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="21">
@@ -922,28 +913,28 @@
         <v>18.0</v>
       </c>
       <c r="B21" t="s">
+        <v>80</v>
+      </c>
+      <c r="C21" t="s">
+        <v>81</v>
+      </c>
+      <c r="D21" t="s">
+        <v>46</v>
+      </c>
+      <c r="E21" t="s">
+        <v>37</v>
+      </c>
+      <c r="F21" t="n">
+        <v>130000.0</v>
+      </c>
+      <c r="G21" t="s">
+        <v>42</v>
+      </c>
+      <c r="H21" t="n">
+        <v>150.0</v>
+      </c>
+      <c r="I21" t="s">
         <v>82</v>
-      </c>
-      <c r="C21" t="s">
-        <v>83</v>
-      </c>
-      <c r="D21" t="s">
-        <v>73</v>
-      </c>
-      <c r="E21" t="s">
-        <v>45</v>
-      </c>
-      <c r="F21" t="n">
-        <v>190000.0</v>
-      </c>
-      <c r="G21" t="s">
-        <v>50</v>
-      </c>
-      <c r="H21" t="n">
-        <v>200.0</v>
-      </c>
-      <c r="I21" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="22">
@@ -951,28 +942,28 @@
         <v>19.0</v>
       </c>
       <c r="B22" t="s">
+        <v>83</v>
+      </c>
+      <c r="C22" t="s">
+        <v>84</v>
+      </c>
+      <c r="D22" t="s">
+        <v>46</v>
+      </c>
+      <c r="E22" t="s">
+        <v>37</v>
+      </c>
+      <c r="F22" t="n">
+        <v>10000.0</v>
+      </c>
+      <c r="G22" t="s">
+        <v>42</v>
+      </c>
+      <c r="H22" t="n">
+        <v>2000.0</v>
+      </c>
+      <c r="I22" t="s">
         <v>85</v>
-      </c>
-      <c r="C22" t="s">
-        <v>86</v>
-      </c>
-      <c r="D22" t="s">
-        <v>73</v>
-      </c>
-      <c r="E22" t="s">
-        <v>45</v>
-      </c>
-      <c r="F22" t="n">
-        <v>240000.0</v>
-      </c>
-      <c r="G22" t="s">
-        <v>50</v>
-      </c>
-      <c r="H22" t="n">
-        <v>100.0</v>
-      </c>
-      <c r="I22" t="s">
-        <v>87</v>
       </c>
     </row>
     <row r="23">
@@ -980,25 +971,25 @@
         <v>20.0</v>
       </c>
       <c r="B23" t="s">
+        <v>86</v>
+      </c>
+      <c r="C23" t="s">
+        <v>87</v>
+      </c>
+      <c r="D23" t="s">
+        <v>46</v>
+      </c>
+      <c r="E23" t="s">
         <v>88</v>
       </c>
-      <c r="C23" t="s">
+      <c r="F23" t="n">
+        <v>60000.0</v>
+      </c>
+      <c r="G23" t="s">
         <v>89</v>
       </c>
-      <c r="D23" t="s">
-        <v>54</v>
-      </c>
-      <c r="E23" t="s">
-        <v>45</v>
-      </c>
-      <c r="F23" t="n">
-        <v>130000.0</v>
-      </c>
-      <c r="G23" t="s">
-        <v>50</v>
-      </c>
       <c r="H23" t="n">
-        <v>150.0</v>
+        <v>100.0</v>
       </c>
       <c r="I23" t="s">
         <v>90</v>
@@ -1015,19 +1006,19 @@
         <v>92</v>
       </c>
       <c r="D24" t="s">
-        <v>54</v>
+        <v>36</v>
       </c>
       <c r="E24" t="s">
-        <v>45</v>
+        <v>88</v>
       </c>
       <c r="F24" t="n">
-        <v>10000.0</v>
+        <v>40000.0</v>
       </c>
       <c r="G24" t="s">
-        <v>50</v>
+        <v>89</v>
       </c>
       <c r="H24" t="n">
-        <v>2000.0</v>
+        <v>100.0</v>
       </c>
       <c r="I24" t="s">
         <v>93</v>
@@ -1044,22 +1035,22 @@
         <v>95</v>
       </c>
       <c r="D25" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="E25" t="s">
+        <v>88</v>
+      </c>
+      <c r="F25" t="n">
+        <v>30000.0</v>
+      </c>
+      <c r="G25" t="s">
+        <v>89</v>
+      </c>
+      <c r="H25" t="n">
+        <v>150.0</v>
+      </c>
+      <c r="I25" t="s">
         <v>96</v>
-      </c>
-      <c r="F25" t="n">
-        <v>60000.0</v>
-      </c>
-      <c r="G25" t="s">
-        <v>97</v>
-      </c>
-      <c r="H25" t="n">
-        <v>100.0</v>
-      </c>
-      <c r="I25" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="26">
@@ -1067,28 +1058,28 @@
         <v>23.0</v>
       </c>
       <c r="B26" t="s">
+        <v>97</v>
+      </c>
+      <c r="C26" t="s">
+        <v>98</v>
+      </c>
+      <c r="D26" t="s">
+        <v>57</v>
+      </c>
+      <c r="E26" t="s">
+        <v>88</v>
+      </c>
+      <c r="F26" t="n">
+        <v>45000.0</v>
+      </c>
+      <c r="G26" t="s">
+        <v>89</v>
+      </c>
+      <c r="H26" t="n">
+        <v>200.0</v>
+      </c>
+      <c r="I26" t="s">
         <v>99</v>
-      </c>
-      <c r="C26" t="s">
-        <v>100</v>
-      </c>
-      <c r="D26" t="s">
-        <v>44</v>
-      </c>
-      <c r="E26" t="s">
-        <v>96</v>
-      </c>
-      <c r="F26" t="n">
-        <v>40000.0</v>
-      </c>
-      <c r="G26" t="s">
-        <v>97</v>
-      </c>
-      <c r="H26" t="n">
-        <v>100.0</v>
-      </c>
-      <c r="I26" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="27">
@@ -1096,28 +1087,28 @@
         <v>24.0</v>
       </c>
       <c r="B27" t="s">
+        <v>100</v>
+      </c>
+      <c r="C27" t="s">
+        <v>101</v>
+      </c>
+      <c r="D27" t="s">
+        <v>61</v>
+      </c>
+      <c r="E27" t="s">
+        <v>88</v>
+      </c>
+      <c r="F27" t="n">
+        <v>90000.0</v>
+      </c>
+      <c r="G27" t="s">
+        <v>89</v>
+      </c>
+      <c r="H27" t="n">
+        <v>80.0</v>
+      </c>
+      <c r="I27" t="s">
         <v>102</v>
-      </c>
-      <c r="C27" t="s">
-        <v>103</v>
-      </c>
-      <c r="D27" t="s">
-        <v>58</v>
-      </c>
-      <c r="E27" t="s">
-        <v>96</v>
-      </c>
-      <c r="F27" t="n">
-        <v>30000.0</v>
-      </c>
-      <c r="G27" t="s">
-        <v>97</v>
-      </c>
-      <c r="H27" t="n">
-        <v>150.0</v>
-      </c>
-      <c r="I27" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="28">
@@ -1125,28 +1116,28 @@
         <v>25.0</v>
       </c>
       <c r="B28" t="s">
+        <v>103</v>
+      </c>
+      <c r="C28" t="s">
+        <v>104</v>
+      </c>
+      <c r="D28" t="s">
         <v>105</v>
       </c>
-      <c r="C28" t="s">
-        <v>106</v>
-      </c>
-      <c r="D28" t="s">
-        <v>65</v>
-      </c>
       <c r="E28" t="s">
-        <v>96</v>
+        <v>19</v>
       </c>
       <c r="F28" t="n">
-        <v>45000.0</v>
+        <v>50000.0</v>
       </c>
       <c r="G28" t="s">
-        <v>97</v>
+        <v>32</v>
       </c>
       <c r="H28" t="n">
-        <v>200.0</v>
+        <v>199.0</v>
       </c>
       <c r="I28" t="s">
-        <v>107</v>
+        <v>51</v>
       </c>
     </row>
     <row r="29">
@@ -1154,28 +1145,28 @@
         <v>26.0</v>
       </c>
       <c r="B29" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C29" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="D29" t="s">
-        <v>69</v>
+        <v>105</v>
       </c>
       <c r="E29" t="s">
-        <v>96</v>
+        <v>13</v>
       </c>
       <c r="F29" t="n">
-        <v>90000.0</v>
+        <v>222.0</v>
       </c>
       <c r="G29" t="s">
-        <v>97</v>
+        <v>42</v>
       </c>
       <c r="H29" t="n">
-        <v>80.0</v>
+        <v>22.0</v>
       </c>
       <c r="I29" t="s">
-        <v>110</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>